<commit_message>
added sarima forecast impacts
</commit_message>
<xml_diff>
--- a/Impact/Improvement Metrics - Across All Projects.xlsx
+++ b/Impact/Improvement Metrics - Across All Projects.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inspirewellness-my.sharepoint.com/personal/sburi_humana_com/Documents/Documents/My Files/Python/CustomEnv/Work Impact/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inspirewellness-my.sharepoint.com/personal/sburi_humana_com/Documents/Documents/My Files/Python/CustomEnv/Impact/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="257" documentId="8_{0B40D6D4-65E6-4A7A-AF4C-BE61588FAE02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F93A97D-20B5-4B0D-88C1-9FE5932FA02A}"/>
+  <xr:revisionPtr revIDLastSave="313" documentId="8_{0B40D6D4-65E6-4A7A-AF4C-BE61588FAE02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B674250-A4B4-4FA0-B0F0-1D132DB46775}"/>
   <bookViews>
-    <workbookView xWindow="34290" yWindow="-110" windowWidth="20700" windowHeight="11140" activeTab="2" xr2:uid="{BBA7550B-BEA3-4F64-81C9-D66EB43BF2E3}"/>
+    <workbookView xWindow="34290" yWindow="-110" windowWidth="20700" windowHeight="11140" activeTab="3" xr2:uid="{BBA7550B-BEA3-4F64-81C9-D66EB43BF2E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Budget" sheetId="2" r:id="rId1"/>
     <sheet name="Budget backups" sheetId="3" r:id="rId2"/>
     <sheet name="Contract Classifier" sheetId="1" r:id="rId3"/>
+    <sheet name="Sarima Forecast" sheetId="5" r:id="rId4"/>
+    <sheet name="Sarima Forecast Backups" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="66">
   <si>
     <t>Steven Buri</t>
   </si>
@@ -160,6 +162,81 @@
   </si>
   <si>
     <t>Decreased Budget Management Cost</t>
+  </si>
+  <si>
+    <t>Sep YTD Actuals</t>
+  </si>
+  <si>
+    <t>Sep YTD Mean Validation</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>Variance %</t>
+  </si>
+  <si>
+    <t>Original Forecast</t>
+  </si>
+  <si>
+    <t>Original Sep YTD Forecast</t>
+  </si>
+  <si>
+    <t>Original Forecast per Month</t>
+  </si>
+  <si>
+    <t>Variance Percent</t>
+  </si>
+  <si>
+    <t>Sum Errors</t>
+  </si>
+  <si>
+    <t>Avg. Error</t>
+  </si>
+  <si>
+    <t>Root Error</t>
+  </si>
+  <si>
+    <t>Sum Naïve Errors</t>
+  </si>
+  <si>
+    <t>Avg. Naïve Error</t>
+  </si>
+  <si>
+    <t>Root Naïve Error</t>
+  </si>
+  <si>
+    <t>Naïve Error</t>
+  </si>
+  <si>
+    <t>Current Error</t>
+  </si>
+  <si>
+    <t>Reduction in Error</t>
+  </si>
+  <si>
+    <t>Sarima forecast is 42% better than naïve forecast using mean for validation months</t>
+  </si>
+  <si>
+    <t>Sarima forecast is 93% better than our forecast was in Feb, Jan-Sep Forecast.</t>
+  </si>
+  <si>
+    <t>Original Risk</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Med</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>New Risk</t>
+  </si>
+  <si>
+    <t>Risk Improvement</t>
   </si>
 </sst>
 </file>
@@ -326,7 +403,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -413,6 +490,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1512,6 +1590,283 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>478901</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>61791</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{660D4176-8ED2-4D4C-AF59-9A0B78730720}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="381000" y="2006600"/>
+          <a:ext cx="18995501" cy="10145591"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>65</xdr:col>
+      <xdr:colOff>418575</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>96720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FD93875-4B89-4FEE-A5A3-D6097FFDCC33}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21056600" y="2006600"/>
+          <a:ext cx="18985975" cy="10536120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>67</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>98</xdr:col>
+      <xdr:colOff>532869</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>10994</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66F0BF37-DCFD-485A-8CF5-71BDD18DD93D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="41325800" y="2108200"/>
+          <a:ext cx="18947869" cy="10526594"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>209017</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>33226</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD94FB2D-2CDC-4DA1-B523-77F6249CCD41}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="787400" y="13639800"/>
+          <a:ext cx="18928817" cy="10574226"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>339100</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>48429</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5772D904-D74F-45E1-9E48-61A770769BEA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21082000" y="14198600"/>
+          <a:ext cx="18271500" cy="5763429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>65</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>69</xdr:col>
+      <xdr:colOff>340088</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>130530</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD6463DB-C98F-4CF4-9807-6C130D2BB677}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="39801800" y="14300200"/>
+          <a:ext cx="2600688" cy="2543530"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -2239,7 +2594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDBBC0B4-B4C9-49F9-A9C5-739CA73257C1}">
   <dimension ref="B2:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -2354,4 +2709,267 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{142668EA-B209-497F-9FB1-EC41800A32F0}">
+  <dimension ref="A2:K17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="7" max="7" width="16.90625" customWidth="1"/>
+    <col min="8" max="8" width="24.08984375" customWidth="1"/>
+    <col min="10" max="10" width="16.7265625" customWidth="1"/>
+    <col min="11" max="11" width="13.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="27">
+        <v>14229000</v>
+      </c>
+      <c r="G2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="27">
+        <v>508786170882.57745</v>
+      </c>
+      <c r="J2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="27">
+        <v>14668000</v>
+      </c>
+      <c r="G3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="27">
+        <v>50878617088.257744</v>
+      </c>
+      <c r="J3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" s="27">
+        <v>13400000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B4" s="27"/>
+      <c r="G4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="27">
+        <v>225562.88943054827</v>
+      </c>
+      <c r="J4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4" s="27">
+        <v>10400000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="27">
+        <f>B3-B2</f>
+        <v>439000</v>
+      </c>
+      <c r="H5" s="27"/>
+      <c r="J5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" s="27">
+        <v>7400000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="32">
+        <f>B5/B2</f>
+        <v>3.0852484362920797E-2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="27">
+        <v>1535193236458.573</v>
+      </c>
+      <c r="K6" s="27"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="27">
+        <v>153519323645.8573</v>
+      </c>
+      <c r="J7" t="s">
+        <v>64</v>
+      </c>
+      <c r="K7" s="27"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="27">
+        <v>391815.42037783214</v>
+      </c>
+      <c r="J8" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8" s="27">
+        <v>2900000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H9" s="27"/>
+      <c r="J9" t="s">
+        <v>62</v>
+      </c>
+      <c r="K9" s="27">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="27">
+        <v>37200000</v>
+      </c>
+      <c r="H10" s="27"/>
+      <c r="J10" t="s">
+        <v>63</v>
+      </c>
+      <c r="K10" s="27">
+        <v>3100000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="27">
+        <f>B10/12</f>
+        <v>3100000</v>
+      </c>
+      <c r="G11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="27">
+        <v>391815.42037783214</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="27">
+        <f>B11*9</f>
+        <v>27900000</v>
+      </c>
+      <c r="G12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12" s="27">
+        <v>225562.88943054827</v>
+      </c>
+      <c r="J12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B13" s="27"/>
+      <c r="G13" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" s="32">
+        <v>-0.42431339426856818</v>
+      </c>
+      <c r="J13" t="s">
+        <v>61</v>
+      </c>
+      <c r="K13" s="32">
+        <f>(K8-K3)/K3</f>
+        <v>-0.78358208955223885</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="27">
+        <f>B12-B2</f>
+        <v>13671000</v>
+      </c>
+      <c r="J14" t="s">
+        <v>62</v>
+      </c>
+      <c r="K14" s="32">
+        <f t="shared" ref="K14:K15" si="0">(K9-K4)/K4</f>
+        <v>-0.99519230769230771</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="32">
+        <f>B14/B2</f>
+        <v>0.96078431372549022</v>
+      </c>
+      <c r="G15" t="s">
+        <v>58</v>
+      </c>
+      <c r="J15" t="s">
+        <v>63</v>
+      </c>
+      <c r="K15" s="32">
+        <f t="shared" si="0"/>
+        <v>-0.58108108108108103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6BD1C1E-1011-4EB9-B287-B5D386B34ADE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A37" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="BU112" sqref="BU111:BU112"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added metrics on sarima forecast
</commit_message>
<xml_diff>
--- a/Impact/Improvement Metrics - Across All Projects.xlsx
+++ b/Impact/Improvement Metrics - Across All Projects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inspirewellness-my.sharepoint.com/personal/sburi_humana_com/Documents/Documents/My Files/Python/CustomEnv/Impact/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="321" documentId="8_{0B40D6D4-65E6-4A7A-AF4C-BE61588FAE02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13F4B14C-3762-44ED-8B47-DD4192D4D0B2}"/>
+  <xr:revisionPtr revIDLastSave="416" documentId="8_{0B40D6D4-65E6-4A7A-AF4C-BE61588FAE02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED51527C-3CDC-4544-B19A-B8BE3B8D0C9F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{BBA7550B-BEA3-4F64-81C9-D66EB43BF2E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" activeTab="4" xr2:uid="{BBA7550B-BEA3-4F64-81C9-D66EB43BF2E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Budget" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="79">
   <si>
     <t>Steven Buri</t>
   </si>
@@ -237,6 +237,45 @@
   <si>
     <t xml:space="preserve">From "Processed_ForecastandActuals" 9/15/22. Multiplied 4,386 rows by by 3 for Forecast, Actuals, and Variances.
 Added "BudgetDistributions_Main" 9/15/22 with 993 to account for budget information as well. </t>
+  </si>
+  <si>
+    <t>Automated DL Inputs</t>
+  </si>
+  <si>
+    <t>Manual DL Inputs</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>From CECP Forecast</t>
+  </si>
+  <si>
+    <t>From CECP Forecast, includes forecast months</t>
+  </si>
+  <si>
+    <t>DL Inputs Automated</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Prior Script Count</t>
+  </si>
+  <si>
+    <t>Current Script Count</t>
+  </si>
+  <si>
+    <t>Reduction in required scripts needed</t>
+  </si>
+  <si>
+    <t>Forecast Prediction, based on prediction Feb-Dec of 2022</t>
+  </si>
+  <si>
+    <t>Actual Results</t>
+  </si>
+  <si>
+    <t>Sarima Forecast Accuracy</t>
   </si>
 </sst>
 </file>
@@ -409,7 +448,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -500,12 +539,125 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="65">
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1884,85 +2036,111 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0AE75F34-76B8-4ABB-9EA2-1EF5A6FB3364}" name="Table1" displayName="Table1" ref="A1:B6" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0AE75F34-76B8-4ABB-9EA2-1EF5A6FB3364}" name="Table1" displayName="Table1" ref="A1:B6" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
   <autoFilter ref="A1:B6" xr:uid="{0AE75F34-76B8-4ABB-9EA2-1EF5A6FB3364}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{84CEBBF1-AC5E-41C8-8049-FD144B0ADE50}" name="Query" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{5385DC53-2B7D-41CD-9F00-295AAE587E31}" name="Metric" dataDxfId="48" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{84CEBBF1-AC5E-41C8-8049-FD144B0ADE50}" name="Query" dataDxfId="62"/>
+    <tableColumn id="2" xr3:uid="{5385DC53-2B7D-41CD-9F00-295AAE587E31}" name="Metric" dataDxfId="61" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{58E337BD-7A79-497A-85AF-FAD81B190DC3}" name="Table2" displayName="Table2" ref="D1:F3" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{58E337BD-7A79-497A-85AF-FAD81B190DC3}" name="Table2" displayName="Table2" ref="D1:F3" totalsRowShown="0" headerRowDxfId="60" dataDxfId="58" headerRowBorderDxfId="59" tableBorderDxfId="57" totalsRowBorderDxfId="56">
   <autoFilter ref="D1:F3" xr:uid="{58E337BD-7A79-497A-85AF-FAD81B190DC3}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{07AD9632-FD9A-4D7F-95DE-63CE76BD8ECC}" name="Increased Visibility" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{9E168082-D05F-47C9-9004-F2AAED5F24F6}" name="Metric" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{5B1795B7-B20F-4005-A2E9-78F7530AA574}" name="Notes" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{07AD9632-FD9A-4D7F-95DE-63CE76BD8ECC}" name="Increased Visibility" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{9E168082-D05F-47C9-9004-F2AAED5F24F6}" name="Metric" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{5B1795B7-B20F-4005-A2E9-78F7530AA574}" name="Notes" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0DBFCBAE-B46A-4EC2-9EF1-59960A831D4B}" name="Table24" displayName="Table24" ref="H1:J3" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36" totalsRowBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0DBFCBAE-B46A-4EC2-9EF1-59960A831D4B}" name="Table24" displayName="Table24" ref="H1:J3" totalsRowShown="0" headerRowDxfId="52" dataDxfId="50" headerRowBorderDxfId="51" tableBorderDxfId="49" totalsRowBorderDxfId="48">
   <autoFilter ref="H1:J3" xr:uid="{0DBFCBAE-B46A-4EC2-9EF1-59960A831D4B}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{89E6102F-F156-4701-9B18-F56A8DE43623}" name="Reduced Underspend/Overspend" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{92A9C58F-D62E-4057-A20D-0699DC7490AD}" name="Metric" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{4D037B42-992E-4B05-A268-A86045066E9B}" name="Notes" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{89E6102F-F156-4701-9B18-F56A8DE43623}" name="Reduced Underspend/Overspend" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{92A9C58F-D62E-4057-A20D-0699DC7490AD}" name="Metric" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{4D037B42-992E-4B05-A268-A86045066E9B}" name="Notes" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1B270726-04DD-4554-B779-CE4538414360}" name="Table25" displayName="Table25" ref="L1:N3" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1B270726-04DD-4554-B779-CE4538414360}" name="Table25" displayName="Table25" ref="L1:N3" totalsRowShown="0" headerRowDxfId="44" dataDxfId="42" headerRowBorderDxfId="43" tableBorderDxfId="41" totalsRowBorderDxfId="40">
   <autoFilter ref="L1:N3" xr:uid="{1B270726-04DD-4554-B779-CE4538414360}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{43754167-7C12-480B-8B0F-AC470CB179C0}" name="Increased Report Creation Speed" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{CABD709F-B5C1-472D-926F-019CEB937CD2}" name="Metric" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{4A2DF080-D579-44D3-BA1B-9BE812BC7E6E}" name="Notes" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{43754167-7C12-480B-8B0F-AC470CB179C0}" name="Increased Report Creation Speed" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{CABD709F-B5C1-472D-926F-019CEB937CD2}" name="Metric" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{4A2DF080-D579-44D3-BA1B-9BE812BC7E6E}" name="Notes" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0EE52BEF-63D4-4F8E-96F2-033D59D45715}" name="Table26" displayName="Table26" ref="T1:V3" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20" totalsRowBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0EE52BEF-63D4-4F8E-96F2-033D59D45715}" name="Table26" displayName="Table26" ref="T1:V3" totalsRowShown="0" headerRowDxfId="36" dataDxfId="34" headerRowBorderDxfId="35" tableBorderDxfId="33" totalsRowBorderDxfId="32">
   <autoFilter ref="T1:V3" xr:uid="{0EE52BEF-63D4-4F8E-96F2-033D59D45715}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{59BAF2A8-087F-4444-945C-04765696349E}" name="Variances Requiring Touchpoints" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{271B9954-B2A3-4E22-8B68-352D30531BB7}" name="Metric" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{4C854EE8-9734-40ED-8BA5-2057838617A9}" name="Notes" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{59BAF2A8-087F-4444-945C-04765696349E}" name="Variances Requiring Touchpoints" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{271B9954-B2A3-4E22-8B68-352D30531BB7}" name="Metric" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{4C854EE8-9734-40ED-8BA5-2057838617A9}" name="Notes" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AD2F7457-8C4E-48C1-80D1-D0653326DA82}" name="Table6" displayName="Table6" ref="X1:Z3" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{AD2F7457-8C4E-48C1-80D1-D0653326DA82}" name="Table6" displayName="Table6" ref="X1:Z3" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25" totalsRowBorderDxfId="24">
   <autoFilter ref="X1:Z3" xr:uid="{AD2F7457-8C4E-48C1-80D1-D0653326DA82}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1776EA5E-1F77-4A3C-8ACC-4AA80D2B4570}" name="YoY Variance" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{A4ED0614-EB8B-4957-9D34-5DF120062FAD}" name="Metric" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{1776EA5E-1F77-4A3C-8ACC-4AA80D2B4570}" name="YoY Variance" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{A4ED0614-EB8B-4957-9D34-5DF120062FAD}" name="Metric" dataDxfId="22">
       <calculatedColumnFormula>20004141 / 17850000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{CE05403B-5268-42D2-8032-1292226DAA3C}" name="Notes" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{CE05403B-5268-42D2-8032-1292226DAA3C}" name="Notes" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{92035B57-C667-4DFA-927C-50AC4F14B00D}" name="Table2510" displayName="Table2510" ref="P1:R3" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{92035B57-C667-4DFA-927C-50AC4F14B00D}" name="Table2510" displayName="Table2510" ref="P1:R3" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="P1:R3" xr:uid="{92035B57-C667-4DFA-927C-50AC4F14B00D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0DC566FE-AD34-40D8-8547-586F2C5A4662}" name="Decreased Costs" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{1D1F2F33-7DF9-4506-BEF0-45233F3330FE}" name="Metric" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{A0B226A4-4743-4F6E-B770-00F27953236D}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{0DC566FE-AD34-40D8-8547-586F2C5A4662}" name="Decreased Costs" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{1D1F2F33-7DF9-4506-BEF0-45233F3330FE}" name="Metric" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{A0B226A4-4743-4F6E-B770-00F27953236D}" name="Notes" dataDxfId="13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{F21DA81E-1531-49B8-BE34-CD2D010E25A2}" name="Table7" displayName="Table7" ref="AB1:AD3" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="AB1:AD3" xr:uid="{F21DA81E-1531-49B8-BE34-CD2D010E25A2}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{9131DD34-0525-42B2-B835-363673C0FFD6}" name="Type" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{04437AFB-88E4-45A7-A279-EDA86599E3C4}" name="Metric" dataDxfId="6">
+      <calculatedColumnFormula>11+24</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{C55E199F-D6F7-4EC4-A77A-4EACB7935E27}" name="Notes" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{2048AF6F-C8A2-4FA2-8722-CAE9B47CCBD9}" name="Table8" displayName="Table8" ref="AF1:AH3" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="AF1:AH3" xr:uid="{2048AF6F-C8A2-4FA2-8722-CAE9B47CCBD9}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{11CDF052-77AC-4A68-A463-88CF343DBFCE}" name="Title" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{82D1AE67-80D8-447C-8B52-A3A96BEF7B3B}" name="Metric" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{7B2E64D1-BD48-4C5E-A495-3FAF9E3A8FBE}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2265,10 +2443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63ED5C62-F45C-44A2-8E29-37096EA35BAB}">
-  <dimension ref="A1:Z10"/>
+  <dimension ref="A1:AH10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView showGridLines="0" topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD9" sqref="AD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2287,10 +2465,14 @@
     <col min="18" max="18" width="35.1796875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="30.7265625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="32.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="68.36328125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="39.6328125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="31.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -2352,8 +2534,26 @@
       <c r="Z1" s="13" t="s">
         <v>24</v>
       </c>
+      <c r="AB1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC1" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:26" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -2421,8 +2621,24 @@
       <c r="Z2" s="21" t="s">
         <v>36</v>
       </c>
+      <c r="AB2" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC2" s="34">
+        <v>8</v>
+      </c>
+      <c r="AD2" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>12</v>
+      </c>
+      <c r="AH2" s="1"/>
     </row>
-    <row r="3" spans="1:26" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:34" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -2482,10 +2698,31 @@
       <c r="X3" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="Y3" s="25"/>
+      <c r="Y3" s="25">
+        <f>ABS(18688166/20505605-1)</f>
+        <v>8.8631327873525345E-2</v>
+      </c>
       <c r="Z3" s="23"/>
+      <c r="AB3" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC3" s="32">
+        <f t="shared" ref="AC3" si="0">11+24</f>
+        <v>35</v>
+      </c>
+      <c r="AD3" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG3" s="1">
+        <f>7+0</f>
+        <v>7</v>
+      </c>
+      <c r="AH3" s="1"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -2494,7 +2731,7 @@
         <v>-0.86933333333333329</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>39</v>
       </c>
@@ -2548,11 +2785,27 @@
       </c>
       <c r="Y5" s="16">
         <f>(Y3-Y2)/Y2</f>
-        <v>-1</v>
+        <v>-0.26556840868706971</v>
       </c>
       <c r="Z5" s="15"/>
+      <c r="AB5" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC5" s="16">
+        <f>AC3/SUM(Table7[Metric])</f>
+        <v>0.81395348837209303</v>
+      </c>
+      <c r="AD5" s="15"/>
+      <c r="AF5" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG5" s="16">
+        <f>AG3/SUM(Table8[Metric])-1</f>
+        <v>-0.63157894736842102</v>
+      </c>
+      <c r="AH5" s="15"/>
     </row>
-    <row r="6" spans="1:26" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:34" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -2565,14 +2818,14 @@
         <v>65200</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
       <c r="I10" s="26"/>
       <c r="V10" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="7">
+  <tableParts count="9">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -2580,6 +2833,8 @@
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2605,7 +2860,7 @@
   <dimension ref="B2:L9"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H7" sqref="B4:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2723,10 +2978,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{142668EA-B209-497F-9FB1-EC41800A32F0}">
-  <dimension ref="A2:K17"/>
+  <dimension ref="A2:N17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2737,9 +2992,11 @@
     <col min="8" max="8" width="24.08984375" customWidth="1"/>
     <col min="10" max="10" width="16.7265625" customWidth="1"/>
     <col min="11" max="11" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="48.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -2755,8 +3012,14 @@
       <c r="J2" t="s">
         <v>59</v>
       </c>
+      <c r="M2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -2775,8 +3038,14 @@
       <c r="K3" s="26">
         <v>13400000</v>
       </c>
+      <c r="M3" t="s">
+        <v>76</v>
+      </c>
+      <c r="N3" s="26">
+        <v>18619428</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B4" s="26"/>
       <c r="G4" t="s">
         <v>50</v>
@@ -2790,8 +3059,14 @@
       <c r="K4" s="26">
         <v>10400000</v>
       </c>
+      <c r="M4" t="s">
+        <v>77</v>
+      </c>
+      <c r="N4" s="26">
+        <v>18688165.6895</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -2806,8 +3081,15 @@
       <c r="K5" s="26">
         <v>7400000</v>
       </c>
+      <c r="M5" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" s="26">
+        <f>N4-N3</f>
+        <v>68737.689500000328</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -2823,7 +3105,7 @@
       </c>
       <c r="K6" s="26"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G7" t="s">
         <v>52</v>
       </c>
@@ -2834,8 +3116,15 @@
         <v>63</v>
       </c>
       <c r="K7" s="26"/>
+      <c r="M7" t="s">
+        <v>78</v>
+      </c>
+      <c r="N7" s="35">
+        <f>1-(N5/N4)</f>
+        <v>0.99632186001333345</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G8" t="s">
         <v>53</v>
       </c>
@@ -2849,7 +3138,7 @@
         <v>2900000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="H9" s="26"/>
       <c r="J9" t="s">
         <v>61</v>
@@ -2858,7 +3147,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -2873,7 +3162,7 @@
         <v>3100000</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -2888,7 +3177,7 @@
         <v>391815.42037783214</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -2906,7 +3195,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B13" s="26"/>
       <c r="G13" t="s">
         <v>56</v>
@@ -2922,7 +3211,7 @@
         <v>-0.78358208955223885</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -2938,7 +3227,7 @@
         <v>-0.99519230769230771</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -2972,7 +3261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6BD1C1E-1011-4EB9-B287-B5D386B34ADE}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A37" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
       <selection activeCell="BU112" sqref="BU111:BU112"/>
     </sheetView>
   </sheetViews>

</xml_diff>